<commit_message>
Guardar y Editar Viaje, Ya quedo los datos generales y de los Operadores Asignados al Viaje.
</commit_message>
<xml_diff>
--- a/sci/modificaciones 14 Feb.xlsx
+++ b/sci/modificaciones 14 Feb.xlsx
@@ -568,11 +568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:D3"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -597,7 +596,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>44</v>
       </c>
@@ -625,7 +624,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -639,7 +638,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
@@ -653,7 +652,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
@@ -667,7 +666,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -681,7 +680,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>40</v>
       </c>
@@ -695,7 +694,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>47</v>
       </c>
@@ -709,7 +708,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>3</v>
       </c>
@@ -723,7 +722,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>3</v>
       </c>
@@ -737,7 +736,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>3</v>
       </c>
@@ -751,7 +750,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -765,7 +764,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -779,7 +778,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -793,7 +792,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -807,7 +806,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="17" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>61</v>
       </c>
@@ -849,7 +848,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>55</v>
       </c>
@@ -863,7 +862,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>58</v>
       </c>
@@ -877,7 +876,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>58</v>
       </c>
@@ -891,7 +890,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>50</v>
       </c>
@@ -905,7 +904,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>17</v>
       </c>
@@ -919,7 +918,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>17</v>
       </c>
@@ -935,11 +934,6 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:D25">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="Cortes"/>
-      </filters>
-    </filterColumn>
     <sortState ref="A2:D25">
       <sortCondition ref="A1"/>
     </sortState>

</xml_diff>

<commit_message>
Se completo el status del operador en el viaje, up and down.
</commit_message>
<xml_diff>
--- a/sci/modificaciones 14 Feb.xlsx
+++ b/sci/modificaciones 14 Feb.xlsx
@@ -570,8 +570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -751,16 +751,16 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="2" t="s">
         <v>34</v>
       </c>
     </row>
@@ -779,16 +779,16 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="2" t="s">
         <v>39</v>
       </c>
     </row>
@@ -821,16 +821,16 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="2" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Se esta trabajando con los paneles de las fechas, el de gasto ya quedo.
</commit_message>
<xml_diff>
--- a/sci/modificaciones 14 Feb.xlsx
+++ b/sci/modificaciones 14 Feb.xlsx
@@ -571,7 +571,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -611,30 +611,30 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
         <v>30</v>
       </c>
     </row>
@@ -807,16 +807,16 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="2" t="s">
         <v>62</v>
       </c>
     </row>
@@ -835,16 +835,16 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="2" t="s">
         <v>54</v>
       </c>
     </row>
@@ -863,30 +863,30 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="2" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="2" t="s">
         <v>69</v>
       </c>
     </row>

</xml_diff>

<commit_message>
La conexión a la BD se cae.
</commit_message>
<xml_diff>
--- a/sci/modificaciones 14 Feb.xlsx
+++ b/sci/modificaciones 14 Feb.xlsx
@@ -571,7 +571,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="A14" sqref="A14:D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -765,16 +765,16 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="2" t="s">
         <v>37</v>
       </c>
     </row>
@@ -793,16 +793,16 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="2" t="s">
         <v>67</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Ya se agregó los cobros adicionales.
</commit_message>
<xml_diff>
--- a/sci/modificaciones 14 Feb.xlsx
+++ b/sci/modificaciones 14 Feb.xlsx
@@ -571,7 +571,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:D14"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -891,16 +891,16 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A23" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="2" t="s">
         <v>52</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Corrección de errores de la segunda entrega.
</commit_message>
<xml_diff>
--- a/sci/modificaciones 14 Feb.xlsx
+++ b/sci/modificaciones 14 Feb.xlsx
@@ -252,7 +252,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -271,6 +271,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -284,10 +290,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -568,10 +575,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -596,297 +604,297 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+    <row r="9" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+    <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+    <row r="11" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+    <row r="12" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+    <row r="13" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+    <row r="14" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+    <row r="15" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+    <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+    <row r="17" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+    <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+    <row r="19" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="3" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" s="3" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="3" t="s">
         <v>69</v>
       </c>
     </row>
@@ -905,35 +913,42 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" s="3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D25" s="3" t="s">
         <v>22</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:D25">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Viaje -&gt; Operador"/>
+        <filter val="Viaje-&gt;Cobros"/>
+        <filter val="Viajes"/>
+      </filters>
+    </filterColumn>
     <sortState ref="A2:D25">
       <sortCondition ref="A1"/>
     </sortState>

</xml_diff>